<commit_message>
Excel dokoncana vaja 1
</commit_message>
<xml_diff>
--- a/Excel/Vaja1/Listi.xlsx
+++ b/Excel/Vaja1/Listi.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\RP\Excel\Vaja1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gits\RP\Excel\Vaja1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29116D4-7006-4246-8680-30F6F77334F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skladisce" sheetId="1" r:id="rId1"/>
@@ -17,20 +18,29 @@
     <sheet name="Barva" sheetId="4" r:id="rId3"/>
     <sheet name="Padavine" sheetId="3" r:id="rId4"/>
     <sheet name="Mnozenje" sheetId="5" r:id="rId5"/>
-    <sheet name="abc" sheetId="7" r:id="rId6"/>
-    <sheet name="Kovine" sheetId="6" r:id="rId7"/>
+    <sheet name="Kovine" sheetId="6" r:id="rId6"/>
+    <sheet name="Prebivalci" sheetId="8" r:id="rId7"/>
+    <sheet name="Ptice" sheetId="12" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
   <si>
     <t>Datum:</t>
   </si>
@@ -194,19 +204,103 @@
   <si>
     <t>Izkop v tonah</t>
   </si>
+  <si>
+    <t>Cu</t>
+  </si>
+  <si>
+    <t>Zn</t>
+  </si>
+  <si>
+    <t>Pb</t>
+  </si>
+  <si>
+    <t>Au</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>Starost</t>
+  </si>
+  <si>
+    <t>Število preb.</t>
+  </si>
+  <si>
+    <t>Moški</t>
+  </si>
+  <si>
+    <t>Ženske</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>6-10</t>
+  </si>
+  <si>
+    <t>11-15</t>
+  </si>
+  <si>
+    <t>16-20</t>
+  </si>
+  <si>
+    <t>21-30</t>
+  </si>
+  <si>
+    <t>31-40</t>
+  </si>
+  <si>
+    <t>41-50</t>
+  </si>
+  <si>
+    <t>51-60</t>
+  </si>
+  <si>
+    <t>61-70</t>
+  </si>
+  <si>
+    <t>nad 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vrsta</t>
+  </si>
+  <si>
+    <t>Število</t>
+  </si>
+  <si>
+    <t>Ogroženost</t>
+  </si>
+  <si>
+    <t>Sinica</t>
+  </si>
+  <si>
+    <t>Škorec</t>
+  </si>
+  <si>
+    <t>Ščinkavec</t>
+  </si>
+  <si>
+    <t>Vrabec</t>
+  </si>
+  <si>
+    <t>Postovka</t>
+  </si>
+  <si>
+    <t>Skupaj</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="d\.m\.yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="0.00\ &quot;m&quot;"/>
-    <numFmt numFmtId="166" formatCode="0.00\ &quot;m²&quot;"/>
-    <numFmt numFmtId="167" formatCode="0.0\ &quot;kg&quot;"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="d\.m\.yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="0.00\ &quot;m&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00\ &quot;m²&quot;"/>
+    <numFmt numFmtId="168" formatCode="0.0\ &quot;kg&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +341,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -262,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="73">
     <border>
       <left/>
       <right/>
@@ -753,13 +862,452 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -769,7 +1317,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -798,24 +1346,24 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
@@ -841,30 +1389,6 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -906,6 +1430,143 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="68" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="70" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -965,7 +1626,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -991,7 +1651,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sl-SI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1209,7 +1869,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1235,7 +1894,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="sl-SI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1267,7 +1926,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="206273103"/>
@@ -1329,7 +1988,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1355,7 +2013,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="sl-SI"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1387,7 +2045,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="206271791"/>
@@ -1428,7 +2086,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sl-SI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1454,7 +2112,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Izkop kovin</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1480,14 +2162,14 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sl-SI"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="30"/>
-      <c:rotY val="286"/>
+      <c:rotY val="210"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="0"/>
     </c:view3D>
@@ -1542,7 +2224,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:explosion val="60"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -1562,6 +2243,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-474F-40CD-9E06-49C106F9C439}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1582,6 +2268,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-474F-40CD-9E06-49C106F9C439}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1602,6 +2293,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-474F-40CD-9E06-49C106F9C439}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1622,10 +2318,16 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-474F-40CD-9E06-49C106F9C439}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
+            <c:explosion val="24"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
@@ -1642,6 +2344,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-474F-40CD-9E06-49C106F9C439}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1652,7 +2359,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -1670,7 +2377,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="sl-SI"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1696,30 +2403,28 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Kovine!$C$2:$G$2</c:f>
+              <c:f>Kovine!$C$22:$G$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Baker</c:v>
+                  <c:v>Cu</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cink</c:v>
+                  <c:v>Zn</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Svinec</c:v>
+                  <c:v>Pb</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Zlato</c:v>
+                  <c:v>Au</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Železo</c:v>
+                  <c:v>Fe</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1774,8 +2479,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1801,7 +2505,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sl-SI"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1831,7 +2535,974 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sl-SI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sl-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Prebivalci!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Moški</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Prebivalci!$D$2:$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11-15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21-30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31-40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41-50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51-60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61-70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>nad 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Prebivalci!$D$3:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EF44-45CC-87F6-8FBFF87FF895}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Prebivalci!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ženske</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Prebivalci!$D$2:$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11-15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21-30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31-40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41-50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51-60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61-70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>nad 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Prebivalci!$D$4:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EF44-45CC-87F6-8FBFF87FF895}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="489806495"/>
+        <c:axId val="554812799"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="489806495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Starost v letih</a:t>
+                </a:r>
+                <a:endParaRPr lang="sl-SI"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sl-SI"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sl-SI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="554812799"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="554812799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Število</a:t>
+                </a:r>
+                <a:endParaRPr lang="sl-SI"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sl-SI"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sl-SI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="489806495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sl-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sl-SI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Število ptic na opazovanem območju</a:t>
+            </a:r>
+            <a:endParaRPr lang="sl-SI"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sl-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="6"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:explosion val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-CE52-4020-A2C4-B75236C534F0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:explosion val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-CE52-4020-A2C4-B75236C534F0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:explosion val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-CE52-4020-A2C4-B75236C534F0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:explosion val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-CE52-4020-A2C4-B75236C534F0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:explosion val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-CE52-4020-A2C4-B75236C534F0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="sl-SI"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Ptice!$C$2:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Sinica</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Škorec</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ščinkavec</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Vrabec</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Postovka</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Ptice!$C$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE52-4020-A2C4-B75236C534F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="110"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sl-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sl-SI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1922,6 +3593,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
@@ -2935,12 +4686,1034 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>604836</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2948,11 +5721,17 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2974,20 +5753,108 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F1AD72B-A4CC-4FC5-8BF2-58254202C468}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9071684F-C221-4D3B-89D6-7BAEF7CF3406}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3267,7 +6134,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3283,12 +6150,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
@@ -3297,7 +6164,7 @@
       </c>
       <c r="D3" s="5">
         <f ca="1">TODAY()</f>
-        <v>43783</v>
+        <v>43793</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -3406,11 +6273,11 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
       <c r="E11" s="12">
         <f>SUM(E5:E10)</f>
         <v>1669.65</v>
@@ -3427,7 +6294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3808,10 +6675,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -3822,10 +6689,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="48"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -3894,11 +6761,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3954,22 +6821,28 @@
         <v>24</v>
       </c>
       <c r="C4" s="40">
-        <v>9.6799999999999997E-2</v>
+        <f>C3/$E$10</f>
+        <v>9.6774193548387094E-2</v>
       </c>
       <c r="D4" s="40">
-        <v>3.6299999999999999E-2</v>
-      </c>
-      <c r="E4" s="41">
-        <v>4.8399999999999999E-2</v>
+        <f t="shared" ref="D4:H4" si="0">D3/$E$10</f>
+        <v>3.6290322580645164E-2</v>
+      </c>
+      <c r="E4" s="40">
+        <f t="shared" si="0"/>
+        <v>4.8387096774193547E-2</v>
       </c>
       <c r="F4" s="40">
-        <v>0.1694</v>
+        <f t="shared" si="0"/>
+        <v>0.16935483870967741</v>
       </c>
       <c r="G4" s="40">
-        <v>0.129</v>
+        <f t="shared" si="0"/>
+        <v>0.12903225806451613</v>
       </c>
       <c r="H4" s="40">
-        <v>2.8199999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.8225806451612902E-2</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -4026,63 +6899,69 @@
         <v>24</v>
       </c>
       <c r="C8" s="40">
-        <v>1.61E-2</v>
+        <f>C7/$E$10</f>
+        <v>1.6129032258064516E-2</v>
       </c>
       <c r="D8" s="40">
-        <v>6.4500000000000002E-2</v>
+        <f t="shared" ref="D8:H8" si="1">D7/$E$10</f>
+        <v>6.4516129032258063E-2</v>
       </c>
       <c r="E8" s="40">
-        <v>8.0600000000000005E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.0645161290322578E-2</v>
       </c>
       <c r="F8" s="40">
-        <v>9.8599999999999993E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.6774193548387094E-2</v>
       </c>
       <c r="G8" s="40">
-        <v>7.2599999999999998E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.2580645161290328E-2</v>
       </c>
       <c r="H8" s="40">
-        <v>0.1613</v>
+        <f t="shared" si="1"/>
+        <v>0.16129032258064516</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
       <c r="E10" s="34">
         <f>SUM(C7:H7,C3:H3)</f>
         <v>1240</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="34">
         <f>MAX(C3:H3,C7:H7)</f>
         <v>210</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
       <c r="E12" s="34">
         <f>MIN(C3:H3,C7:H7)</f>
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
       <c r="E13" s="34">
         <f>ROUND(AVERAGE(C3:H3,C7:H7),0)</f>
         <v>103</v>
@@ -4101,7 +6980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4112,90 +6991,90 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="54">
+      <c r="C2" s="46">
         <v>1</v>
       </c>
-      <c r="D2" s="55">
+      <c r="D2" s="47">
         <v>2</v>
       </c>
-      <c r="E2" s="56">
+      <c r="E2" s="48">
         <v>3</v>
       </c>
-      <c r="F2" s="55">
+      <c r="F2" s="47">
         <v>4</v>
       </c>
-      <c r="G2" s="56">
+      <c r="G2" s="48">
         <v>5</v>
       </c>
-      <c r="H2" s="55">
+      <c r="H2" s="47">
         <v>6</v>
       </c>
-      <c r="I2" s="56">
+      <c r="I2" s="48">
         <v>7</v>
       </c>
-      <c r="J2" s="55">
+      <c r="J2" s="47">
         <v>8</v>
       </c>
-      <c r="K2" s="57">
+      <c r="K2" s="49">
         <v>9</v>
       </c>
-      <c r="L2" s="52">
+      <c r="L2" s="44">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="60">
+      <c r="B3" s="52">
         <v>1</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="50">
         <f>C$2*$B3</f>
         <v>1</v>
       </c>
-      <c r="D3" s="53">
+      <c r="D3" s="45">
         <f t="shared" ref="D3:L12" si="0">D$2*$B3</f>
         <v>2</v>
       </c>
-      <c r="E3" s="53">
+      <c r="E3" s="45">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="45">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G3" s="53">
+      <c r="G3" s="45">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H3" s="53">
+      <c r="H3" s="45">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I3" s="53">
+      <c r="I3" s="45">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J3" s="53">
+      <c r="J3" s="45">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K3" s="53">
+      <c r="K3" s="45">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L3" s="53">
+      <c r="L3" s="45">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="61">
+      <c r="B4" s="53">
         <v>2</v>
       </c>
-      <c r="C4" s="59">
+      <c r="C4" s="51">
         <f t="shared" ref="C4:C12" si="1">C$2*$B4</f>
         <v>2</v>
       </c>
@@ -4237,10 +7116,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="61">
+      <c r="B5" s="53">
         <v>3</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="51">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -4282,10 +7161,10 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="62">
+      <c r="B6" s="54">
         <v>4</v>
       </c>
-      <c r="C6" s="59">
+      <c r="C6" s="51">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -4327,10 +7206,10 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="61">
+      <c r="B7" s="53">
         <v>5</v>
       </c>
-      <c r="C7" s="59">
+      <c r="C7" s="51">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -4372,10 +7251,10 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="61">
+      <c r="B8" s="53">
         <v>6</v>
       </c>
-      <c r="C8" s="59">
+      <c r="C8" s="51">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -4417,10 +7296,10 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="62">
+      <c r="B9" s="54">
         <v>7</v>
       </c>
-      <c r="C9" s="59">
+      <c r="C9" s="51">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -4462,10 +7341,10 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="61">
+      <c r="B10" s="53">
         <v>8</v>
       </c>
-      <c r="C10" s="59">
+      <c r="C10" s="51">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -4507,10 +7386,10 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="63">
+      <c r="B11" s="55">
         <v>9</v>
       </c>
-      <c r="C11" s="59">
+      <c r="C11" s="51">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -4552,10 +7431,10 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51">
+      <c r="B12" s="43">
         <v>10</v>
       </c>
-      <c r="C12" s="59">
+      <c r="C12" s="51">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -4603,25 +7482,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4635,40 +7500,372 @@
       <c r="B2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="57" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="67">
+      <c r="C3" s="59">
         <v>12000</v>
       </c>
-      <c r="D3" s="67">
+      <c r="D3" s="59">
         <v>11000</v>
       </c>
-      <c r="E3" s="67">
+      <c r="E3" s="59">
         <v>7000</v>
       </c>
-      <c r="F3" s="67">
+      <c r="F3" s="59">
         <v>2000</v>
       </c>
-      <c r="G3" s="67">
+      <c r="G3" s="59">
         <v>25000</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041F417A-88D4-4C0E-992D-6BA926F240F4}">
+  <dimension ref="B1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="74" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="80">
+        <v>100</v>
+      </c>
+      <c r="E3" s="81">
+        <v>150</v>
+      </c>
+      <c r="F3" s="81">
+        <v>140</v>
+      </c>
+      <c r="G3" s="81">
+        <v>160</v>
+      </c>
+      <c r="H3" s="81">
+        <v>140</v>
+      </c>
+      <c r="I3" s="81">
+        <v>100</v>
+      </c>
+      <c r="J3" s="81">
+        <v>80</v>
+      </c>
+      <c r="K3" s="81">
+        <v>60</v>
+      </c>
+      <c r="L3" s="81">
+        <v>80</v>
+      </c>
+      <c r="M3" s="82">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="72"/>
+      <c r="C4" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="83">
+        <v>130</v>
+      </c>
+      <c r="E4" s="84">
+        <v>200</v>
+      </c>
+      <c r="F4" s="84">
+        <v>180</v>
+      </c>
+      <c r="G4" s="84">
+        <v>120</v>
+      </c>
+      <c r="H4" s="84">
+        <v>100</v>
+      </c>
+      <c r="I4" s="84">
+        <v>80</v>
+      </c>
+      <c r="J4" s="84">
+        <v>100</v>
+      </c>
+      <c r="K4" s="84">
+        <v>90</v>
+      </c>
+      <c r="L4" s="84">
+        <v>60</v>
+      </c>
+      <c r="M4" s="85">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="79" t="str">
+        <f>IF(D3&gt;D4,"M","Ž")</f>
+        <v>Ž</v>
+      </c>
+      <c r="E5" s="79" t="str">
+        <f t="shared" ref="E5:M5" si="0">IF(E3&gt;E4,"M","Ž")</f>
+        <v>Ž</v>
+      </c>
+      <c r="F5" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>Ž</v>
+      </c>
+      <c r="G5" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+      <c r="H5" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+      <c r="I5" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+      <c r="J5" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>Ž</v>
+      </c>
+      <c r="K5" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>Ž</v>
+      </c>
+      <c r="L5" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+      <c r="M5" s="79" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2" twoDigitTextYear="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B561DC16-F83A-4A78-A081-40D4C877870B}">
+  <dimension ref="B1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="68"/>
+    </row>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="91" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="92" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="91" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="93" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="94" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="95">
+        <v>405</v>
+      </c>
+      <c r="D3" s="96">
+        <v>150</v>
+      </c>
+      <c r="E3" s="97">
+        <v>70</v>
+      </c>
+      <c r="F3" s="96">
+        <v>220</v>
+      </c>
+      <c r="G3" s="98">
+        <v>17</v>
+      </c>
+      <c r="H3" s="101">
+        <f>SUM(C3:G3)</f>
+        <v>862</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="88" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="102">
+        <f>C3/$H$3</f>
+        <v>0.46983758700696054</v>
+      </c>
+      <c r="D4" s="41">
+        <f t="shared" ref="D4:G4" si="0">D3/$H$3</f>
+        <v>0.1740139211136891</v>
+      </c>
+      <c r="E4" s="103">
+        <f t="shared" si="0"/>
+        <v>8.1206496519721574E-2</v>
+      </c>
+      <c r="F4" s="41">
+        <f t="shared" si="0"/>
+        <v>0.25522041763341069</v>
+      </c>
+      <c r="G4" s="104">
+        <f t="shared" si="0"/>
+        <v>1.9721577726218097E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="99" t="str">
+        <f>IF(C3&lt;100,"da","ne")</f>
+        <v>ne</v>
+      </c>
+      <c r="D5" s="105" t="str">
+        <f t="shared" ref="D5:G5" si="1">IF(D3&lt;100,"da","ne")</f>
+        <v>ne</v>
+      </c>
+      <c r="E5" s="100" t="str">
+        <f t="shared" si="1"/>
+        <v>da</v>
+      </c>
+      <c r="F5" s="105" t="str">
+        <f t="shared" si="1"/>
+        <v>ne</v>
+      </c>
+      <c r="G5" s="106" t="str">
+        <f t="shared" si="1"/>
+        <v>da</v>
       </c>
     </row>
   </sheetData>

</xml_diff>